<commit_message>
Pie in Pie added
</commit_message>
<xml_diff>
--- a/excel/files_11_data_visualization/file01_menu_charts.xlsx
+++ b/excel/files_11_data_visualization/file01_menu_charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjur\OneDrive - Hanzehogeschool Groningen\web_pages\data_analysis\data_analysis\excel\files_11_data_visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hanzenl-my.sharepoint.com/personal/j_hageman_pl_hanze_nl/Documents/web_pages/data_analysis/data_analysis/excel/files_11_data_visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D886B7E1-1ADF-4832-A354-248CA43C74E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D886B7E1-1ADF-4832-A354-248CA43C74E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEDD6AA-4F38-4B97-94CD-D3F9E2094856}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{50F61F0E-0366-4A0C-BD0F-19332FD87CC5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="8" xr2:uid="{50F61F0E-0366-4A0C-BD0F-19332FD87CC5}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="2" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="stacked relative" sheetId="13" r:id="rId6"/>
     <sheet name="pie" sheetId="14" r:id="rId7"/>
     <sheet name="pie_perc" sheetId="15" r:id="rId8"/>
+    <sheet name="pie of pie" sheetId="16" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">menu!$A$1:$X$261</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4188,6 +4189,491 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Relative average amount of calories from fat related to total calories for different food categories</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:ofPieChart>
+        <c:ofPieType val="pie"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>calories from fat</c:v>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3867-4F22-B821-7387C42975C8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pivot table'!$A$4:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Beef &amp; Pork</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Beverages</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Breakfast</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Chicken &amp; Fish</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Coffee &amp; Tea</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Desserts</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Salads</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Smoothies &amp; Shakes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Snacks &amp; Sides</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pivot table'!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>224.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7407407407407407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>248.92857142857142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.22222222222223</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.10526315789474</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>127.67857142857143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.615384615384613</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-3867-4F22-B821-7387C42975C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:splitType val="percent"/>
+        <c:splitPos val="10"/>
+        <c:secondPieSize val="75"/>
+        <c:serLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:serLines>
+      </c:ofPieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4389,6 +4875,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7454,6 +7980,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7684,6 +8715,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFCF5E0A-25AB-41F6-9201-2A6DAE121C4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>168276</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C7E22ED-6092-4AF2-AB8F-FED85E76A407}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -35708,7 +36782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7565106A-8229-4768-A217-3B023C849FD8}">
   <dimension ref="A3:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -35924,8 +36998,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9F99E7-DF8B-4A8E-8F04-DA3137D22D7E}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22446CA8-A947-47FB-9E64-D8CB09A5A429}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>